<commit_message>
caregiving coding and updated spreadsheet of cognitive module states
</commit_message>
<xml_diff>
--- a/data-raw/BRFSS_SGM_CG_COG_States_2015-2017.xlsx
+++ b/data-raw/BRFSS_SGM_CG_COG_States_2015-2017.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcapistrant/Dropbox/BenAnalysis/BRFSS/brrfss/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83C986E3-59AD-5F47-A0C5-377618E3D712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C490D8-426E-F542-81B5-1D73023C7D36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="21600" windowHeight="38400" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
+    <workbookView xWindow="3600" yWindow="460" windowWidth="21600" windowHeight="15940" activeTab="2" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
   </bookViews>
   <sheets>
     <sheet name="Module_States" sheetId="2" r:id="rId1"/>
     <sheet name="SGM_States" sheetId="3" r:id="rId2"/>
     <sheet name="CG_States" sheetId="4" r:id="rId3"/>
     <sheet name="COG_States" sheetId="5" r:id="rId4"/>
+    <sheet name="Covariates" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="295">
   <si>
     <t>Alabama</t>
   </si>
@@ -541,13 +543,385 @@
   </si>
   <si>
     <t>SGM_COG_Any</t>
+  </si>
+  <si>
+    <t>Raw_Variable</t>
+  </si>
+  <si>
+    <t>Which_Analysis</t>
+  </si>
+  <si>
+    <t>New_Variable</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Levels/Range</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>VETERAN3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CIMEMLOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CDHOUSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_MRACE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_RFBING5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_AGE80</t>
+  </si>
+  <si>
+    <t>X_AGE_G</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_AGEG5YR</t>
+  </si>
+  <si>
+    <t>INCOME2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EDUCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PHYSHLTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MENTHLTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ADDEPEV2</t>
+  </si>
+  <si>
+    <t>CHILDREN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EMPLOY1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_SMOKER3</t>
+  </si>
+  <si>
+    <t>X_RFBMI5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_TOTINDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_PSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_STSTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X_LLCPWT</t>
+  </si>
+  <si>
+    <t>Veterans_Cog</t>
+  </si>
+  <si>
+    <t>CIMEMLOS</t>
+  </si>
+  <si>
+    <t>CDHOUSE</t>
+  </si>
+  <si>
+    <t>SEX</t>
+  </si>
+  <si>
+    <t>X_MRACE1</t>
+  </si>
+  <si>
+    <t>X_RFBING5</t>
+  </si>
+  <si>
+    <t>X_AGE80</t>
+  </si>
+  <si>
+    <t>X_AGEG5YR</t>
+  </si>
+  <si>
+    <t>EDUCA</t>
+  </si>
+  <si>
+    <t>MARITAL</t>
+  </si>
+  <si>
+    <t>PHYSHLTH</t>
+  </si>
+  <si>
+    <t>MENTHLTH</t>
+  </si>
+  <si>
+    <t>ADDEPEV2</t>
+  </si>
+  <si>
+    <t>EMPLOY1</t>
+  </si>
+  <si>
+    <t>X_SMOKER3</t>
+  </si>
+  <si>
+    <t>X_TOTINDA</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Veterans</t>
+  </si>
+  <si>
+    <t>Cognitive Fx</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Socioeconomic Status</t>
+  </si>
+  <si>
+    <t>Health Status</t>
+  </si>
+  <si>
+    <t>Health Behaviors</t>
+  </si>
+  <si>
+    <t>Leisure Time Physical Activity</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>Smoking Status</t>
+  </si>
+  <si>
+    <t>Depressive Disorder</t>
+  </si>
+  <si>
+    <t>Mental Health HRQOL</t>
+  </si>
+  <si>
+    <t>Physical Health HRQOL</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Number of Children</t>
+  </si>
+  <si>
+    <t>, Reported, 5-year categories</t>
+  </si>
+  <si>
+    <t>Age, Imputed, 5 year categories</t>
+  </si>
+  <si>
+    <t>Age, Imputed, 5 categories</t>
+  </si>
+  <si>
+    <t>X_RACEGR3</t>
+  </si>
+  <si>
+    <t>SXORIENT</t>
+  </si>
+  <si>
+    <t>HLTHPLN1</t>
+  </si>
+  <si>
+    <t>MEDCOST</t>
+  </si>
+  <si>
+    <t>CHECKUP1</t>
+  </si>
+  <si>
+    <t>X_BMI5CAT</t>
+  </si>
+  <si>
+    <t>X_RFDRHV5</t>
+  </si>
+  <si>
+    <t>X_RFSMOK3</t>
+  </si>
+  <si>
+    <t>HIVRISK</t>
+  </si>
+  <si>
+    <t>TRNSGNDR)</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>HIV Risk</t>
+  </si>
+  <si>
+    <t>Trans HIV</t>
+  </si>
+  <si>
+    <t>Alcohol, Binge Drinking</t>
+  </si>
+  <si>
+    <t>Alcohol, Heavy Drinking</t>
+  </si>
+  <si>
+    <t>Race, imputed 5 level</t>
+  </si>
+  <si>
+    <t>Race, multiple races</t>
+  </si>
+  <si>
+    <t>Doctor Cost Prevented Care</t>
+  </si>
+  <si>
+    <t>Time since last checkup</t>
+  </si>
+  <si>
+    <t>Health Care Coverage (Insurance)</t>
+  </si>
+  <si>
+    <t>CG Flu</t>
+  </si>
+  <si>
+    <t>Caregiving AJPH</t>
+  </si>
+  <si>
+    <t>CG AJPH paper dichotomized at 14+ days</t>
+  </si>
+  <si>
+    <t>Chronic Diseases</t>
+  </si>
+  <si>
+    <t>CG Millennial</t>
+  </si>
+  <si>
+    <t>Time since last dentist visit</t>
+  </si>
+  <si>
+    <t>LASTDEN3</t>
+  </si>
+  <si>
+    <t>Self-Rated Health</t>
+  </si>
+  <si>
+    <t>GENHLTH</t>
+  </si>
+  <si>
+    <t>IMFVPLAC</t>
+  </si>
+  <si>
+    <t>FLUSHOT6</t>
+  </si>
+  <si>
+    <t>Influenza Vaccine - ever?</t>
+  </si>
+  <si>
+    <t>Influenza Vaccine - where?</t>
+  </si>
+  <si>
+    <t>Influenza Vaccine - when?</t>
+  </si>
+  <si>
+    <t>FLSHTMY2</t>
+  </si>
+  <si>
+    <t>Emotional Support</t>
+  </si>
+  <si>
+    <t>EMTSUPRT</t>
+  </si>
+  <si>
+    <t>Life Satisfaction</t>
+  </si>
+  <si>
+    <t>LSATISFY</t>
+  </si>
+  <si>
+    <t>This is in an optional Module</t>
+  </si>
+  <si>
+    <t>https://bmcpublichealth.biomedcentral.com/articles/10.1186/1471-2458-12-685</t>
+  </si>
+  <si>
+    <t>CG AJPH paper has Any of the Following(heart disease, stroke, diabetes, asthma, COPD, Arthritis, or non-skin cancer): CVDCRHD4, CVDSTRK3,DIABETE3,ASTHMA3,CHCOCNCR,CHCCOPD1,HAVARTH3. MCGUIRE et al JHNA 2010 had a count of conditions, too (asthma, arthritis,diabetes,heart disease)</t>
+  </si>
+  <si>
+    <t>SEE NOTE</t>
+  </si>
+  <si>
+    <t>FRUIT2</t>
+  </si>
+  <si>
+    <t>Fruit Intake</t>
+  </si>
+  <si>
+    <t>Vegetable Intake</t>
+  </si>
+  <si>
+    <t>FVGREEN1 and VEGETAB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bmcpublichealth.biomedcentral.com/articles/10.1186/1471-2458-12-685; FVGREEN, FVORANGE, VEGETAB1 in 2015 </t>
+  </si>
+  <si>
+    <t>Maybe only 2015/2017</t>
+  </si>
+  <si>
+    <t>EXERANY2</t>
+  </si>
+  <si>
+    <t>Phyiscal Activity - ever</t>
+  </si>
+  <si>
+    <t>Physical Activity - how often</t>
+  </si>
+  <si>
+    <t>Physical Activity - how long</t>
+  </si>
+  <si>
+    <t>EXEROFT1, EXEROFT2</t>
+  </si>
+  <si>
+    <t>EXERHMM1, EXERHMM2</t>
+  </si>
+  <si>
+    <t>Phyiscal Activity -strengthening</t>
+  </si>
+  <si>
+    <t>STRENGTH</t>
+  </si>
+  <si>
+    <t>Physical Activity is included in the odd years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -594,6 +968,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -612,10 +994,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -626,8 +1009,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -942,7 +1327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FEFCF44-6B25-D842-B032-ED8602B9C853}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
@@ -5778,11 +6163,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34975563-31D7-A243-8C74-D0B76FAAE703}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8947,7 +9332,7 @@
       </c>
       <c r="K34" s="4"/>
       <c r="M34" s="3">
-        <f t="shared" ref="M34:M55" si="2">SUM(D34:J34)</f>
+        <f t="shared" ref="M34:M54" si="2">SUM(D34:J34)</f>
         <v>1</v>
       </c>
       <c r="N34" s="3">
@@ -9648,4 +10033,836 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FC520E-C64D-6242-ADD9-027A4DCE44BD}">
+  <dimension ref="A1:K41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C13" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" t="s">
+        <v>246</v>
+      </c>
+      <c r="K14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" t="s">
+        <v>246</v>
+      </c>
+      <c r="K15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D16" t="s">
+        <v>246</v>
+      </c>
+      <c r="H16" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" t="s">
+        <v>246</v>
+      </c>
+      <c r="H17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" t="s">
+        <v>273</v>
+      </c>
+      <c r="D19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B20" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C21" t="s">
+        <v>279</v>
+      </c>
+      <c r="H21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" t="s">
+        <v>264</v>
+      </c>
+      <c r="C22" t="s">
+        <v>265</v>
+      </c>
+      <c r="D22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" t="s">
+        <v>286</v>
+      </c>
+      <c r="H23" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>223</v>
+      </c>
+      <c r="B24" t="s">
+        <v>288</v>
+      </c>
+      <c r="C24" t="s">
+        <v>290</v>
+      </c>
+      <c r="H24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C26" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B27" t="s">
+        <v>281</v>
+      </c>
+      <c r="C27" t="s">
+        <v>280</v>
+      </c>
+      <c r="H27" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B28" t="s">
+        <v>282</v>
+      </c>
+      <c r="C28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>223</v>
+      </c>
+      <c r="B29" t="s">
+        <v>226</v>
+      </c>
+      <c r="C29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D29" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" t="s">
+        <v>225</v>
+      </c>
+      <c r="C30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" t="s">
+        <v>215</v>
+      </c>
+      <c r="D31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" t="s">
+        <v>250</v>
+      </c>
+      <c r="C32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C33" t="s">
+        <v>242</v>
+      </c>
+      <c r="D33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" t="s">
+        <v>248</v>
+      </c>
+      <c r="C34" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>223</v>
+      </c>
+      <c r="B35" t="s">
+        <v>268</v>
+      </c>
+      <c r="C35" t="s">
+        <v>267</v>
+      </c>
+      <c r="D35" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" t="s">
+        <v>270</v>
+      </c>
+      <c r="C36" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>223</v>
+      </c>
+      <c r="B37" t="s">
+        <v>269</v>
+      </c>
+      <c r="C37" t="s">
+        <v>266</v>
+      </c>
+      <c r="D37" t="s">
+        <v>257</v>
+      </c>
+      <c r="H37" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B38" t="s">
+        <v>256</v>
+      </c>
+      <c r="C38" t="s">
+        <v>238</v>
+      </c>
+      <c r="D38" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>247</v>
+      </c>
+      <c r="B39" t="s">
+        <v>254</v>
+      </c>
+      <c r="C39" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>247</v>
+      </c>
+      <c r="B40" t="s">
+        <v>255</v>
+      </c>
+      <c r="C40" t="s">
+        <v>240</v>
+      </c>
+      <c r="D40" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>247</v>
+      </c>
+      <c r="B41" t="s">
+        <v>262</v>
+      </c>
+      <c r="C41" t="s">
+        <v>263</v>
+      </c>
+      <c r="D41" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H28" r:id="rId1" xr:uid="{00B99229-3D0B-AA4C-B75B-579013D173A6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6487BB6-B0C6-6B4C-B183-F3036D1DD1C9}">
+  <dimension ref="A1:W19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L1" t="s">
+        <v>188</v>
+      </c>
+      <c r="M1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" t="s">
+        <v>191</v>
+      </c>
+      <c r="P1" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>193</v>
+      </c>
+      <c r="R1" t="s">
+        <v>194</v>
+      </c>
+      <c r="S1" t="s">
+        <v>195</v>
+      </c>
+      <c r="T1" t="s">
+        <v>196</v>
+      </c>
+      <c r="U1" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1" t="s">
+        <v>198</v>
+      </c>
+      <c r="W1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I2" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K2" t="s">
+        <v>237</v>
+      </c>
+      <c r="L2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M2" t="s">
+        <v>239</v>
+      </c>
+      <c r="N2" t="s">
+        <v>240</v>
+      </c>
+      <c r="O2" t="s">
+        <v>241</v>
+      </c>
+      <c r="P2" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>211</v>
+      </c>
+      <c r="R2" t="s">
+        <v>242</v>
+      </c>
+      <c r="S2" t="s">
+        <v>243</v>
+      </c>
+      <c r="T2" t="s">
+        <v>244</v>
+      </c>
+      <c r="U2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New variable Coding and corresponding spreadsheet
</commit_message>
<xml_diff>
--- a/data-raw/BRFSS_SGM_CG_COG_States_2015-2017.xlsx
+++ b/data-raw/BRFSS_SGM_CG_COG_States_2015-2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcapistrant/Dropbox/BenAnalysis/BRFSS/brrfss/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Dropbox/BenAnalysis/BRFSS/brrfss/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C490D8-426E-F542-81B5-1D73023C7D36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9A0D64-ABAE-FF4C-9052-8E5A3200D92F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="460" windowWidth="21600" windowHeight="15940" activeTab="2" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="21600" windowHeight="15940" activeTab="4" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
   </bookViews>
   <sheets>
     <sheet name="Module_States" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Covariates" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="319">
   <si>
     <t>Alabama</t>
   </si>
@@ -653,9 +653,6 @@
     <t>X_AGE80</t>
   </si>
   <si>
-    <t>X_AGEG5YR</t>
-  </si>
-  <si>
     <t>EDUCA</t>
   </si>
   <si>
@@ -731,15 +728,9 @@
     <t>Number of Children</t>
   </si>
   <si>
-    <t>, Reported, 5-year categories</t>
-  </si>
-  <si>
     <t>Age, Imputed, 5 year categories</t>
   </si>
   <si>
-    <t>Age, Imputed, 5 categories</t>
-  </si>
-  <si>
     <t>X_RACEGR3</t>
   </si>
   <si>
@@ -915,6 +906,87 @@
   </si>
   <si>
     <t>Physical Activity is included in the odd years</t>
+  </si>
+  <si>
+    <t>Employment Status</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>need to change trans hiv</t>
+  </si>
+  <si>
+    <t>age_num</t>
+  </si>
+  <si>
+    <t>numeric, quantiative</t>
+  </si>
+  <si>
+    <t>age_cat</t>
+  </si>
+  <si>
+    <t>factor, categorical</t>
+  </si>
+  <si>
+    <t>5-year age categories (18-24, 25-29,…95-99)</t>
+  </si>
+  <si>
+    <t>18-99</t>
+  </si>
+  <si>
+    <t>sex_d_fct</t>
+  </si>
+  <si>
+    <t>factor, dichotomous</t>
+  </si>
+  <si>
+    <t>female/male</t>
+  </si>
+  <si>
+    <t>millennial_d_num</t>
+  </si>
+  <si>
+    <t>numeric, dichotomous</t>
+  </si>
+  <si>
+    <t>1/0</t>
+  </si>
+  <si>
+    <t>millennial_d_fct</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>agege45_d_num</t>
+  </si>
+  <si>
+    <t>agege45_d_fct</t>
+  </si>
+  <si>
+    <t>Millennial defined as born between 1981-1996, per Pew Research http://www.pewresearch.org/fact-tank/2018/03/01/defining-generations-where-millennials-end-and-post-millennials-begin/</t>
+  </si>
+  <si>
+    <t>45+ received the cognitive module</t>
+  </si>
+  <si>
+    <t>CG SGM</t>
+  </si>
+  <si>
+    <t>Aging journals will want 65+</t>
+  </si>
+  <si>
+    <t>agege65_d_num</t>
+  </si>
+  <si>
+    <t>agege65_d_fct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For </t>
   </si>
 </sst>
 </file>
@@ -998,7 +1070,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1010,6 +1082,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6163,7 +6236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34975563-31D7-A243-8C74-D0B76FAAE703}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10037,252 +10110,363 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FC520E-C64D-6242-ADD9-027A4DCE44BD}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>219</v>
       </c>
-      <c r="B1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>220</v>
-      </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2" t="s">
+        <v>301</v>
+      </c>
+      <c r="H2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D3" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+      <c r="E4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F4" t="s">
+        <v>306</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="H4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+      <c r="E5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="H5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="C6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D6" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="H6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="D7" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+      <c r="E7" t="s">
+        <v>311</v>
+      </c>
+      <c r="F7" t="s">
+        <v>303</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="H7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C8" t="s">
         <v>206</v>
       </c>
       <c r="D8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+      <c r="E8" t="s">
+        <v>316</v>
+      </c>
+      <c r="F8" t="s">
+        <v>306</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="H8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="D9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+      <c r="E9" t="s">
+        <v>317</v>
+      </c>
+      <c r="F9" t="s">
+        <v>303</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="H9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B11" t="s">
         <v>231</v>
       </c>
       <c r="C11" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C12" t="s">
-        <v>192</v>
-      </c>
-      <c r="D12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="B13" t="s">
+        <v>250</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D13" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="B14" t="s">
+        <v>229</v>
       </c>
       <c r="C14" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>246</v>
-      </c>
-      <c r="K14" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+      <c r="E14" t="s">
+        <v>302</v>
+      </c>
+      <c r="F14" t="s">
+        <v>303</v>
+      </c>
+      <c r="G14" t="s">
+        <v>304</v>
+      </c>
+      <c r="H14" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="B15" t="s">
+        <v>216</v>
       </c>
       <c r="C15" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
-        <v>246</v>
-      </c>
-      <c r="K15" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>222</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="C16" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D16" t="s">
-        <v>246</v>
-      </c>
-      <c r="H16" t="s">
-        <v>259</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -10290,16 +10474,13 @@
         <v>222</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="C17" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="D17" t="s">
         <v>246</v>
-      </c>
-      <c r="H17" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -10307,13 +10488,13 @@
         <v>222</v>
       </c>
       <c r="B18" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C18" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="D18" t="s">
-        <v>200</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -10321,13 +10502,13 @@
         <v>222</v>
       </c>
       <c r="B19" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C19" t="s">
-        <v>273</v>
-      </c>
-      <c r="D19" t="s">
-        <v>261</v>
+        <v>277</v>
+      </c>
+      <c r="H19" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -10335,13 +10516,13 @@
         <v>222</v>
       </c>
       <c r="B20" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="C20" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="D20" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -10349,13 +10530,13 @@
         <v>222</v>
       </c>
       <c r="B21" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C21" t="s">
-        <v>279</v>
-      </c>
-      <c r="H21" t="s">
-        <v>278</v>
+        <v>264</v>
+      </c>
+      <c r="D21" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -10363,281 +10544,367 @@
         <v>222</v>
       </c>
       <c r="B22" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D22" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B23" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="C23" t="s">
-        <v>286</v>
+        <v>263</v>
+      </c>
+      <c r="D23" t="s">
+        <v>254</v>
       </c>
       <c r="H23" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" t="s">
         <v>223</v>
       </c>
-      <c r="B24" t="s">
-        <v>288</v>
-      </c>
       <c r="C24" t="s">
-        <v>290</v>
-      </c>
-      <c r="H24" t="s">
-        <v>294</v>
+        <v>214</v>
+      </c>
+      <c r="D24" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B25" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C25" t="s">
-        <v>291</v>
+        <v>283</v>
+      </c>
+      <c r="H25" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B26" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C26" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B27" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C27" t="s">
-        <v>280</v>
-      </c>
-      <c r="H27" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B28" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C28" t="s">
-        <v>283</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>284</v>
+        <v>287</v>
+      </c>
+      <c r="H28" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D29" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B30" t="s">
-        <v>225</v>
+        <v>279</v>
       </c>
       <c r="C30" t="s">
-        <v>195</v>
-      </c>
-      <c r="D30" t="s">
-        <v>246</v>
+        <v>280</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="B31" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="C31" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="D31" t="s">
-        <v>200</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="B32" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C32" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="D32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>244</v>
+      </c>
+      <c r="B33" t="s">
+        <v>252</v>
+      </c>
+      <c r="C33" t="s">
+        <v>237</v>
+      </c>
+      <c r="D33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>244</v>
+      </c>
+      <c r="B34" t="s">
+        <v>259</v>
+      </c>
+      <c r="C34" t="s">
+        <v>260</v>
+      </c>
+      <c r="D34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>221</v>
+      </c>
+      <c r="B35" t="s">
+        <v>257</v>
+      </c>
+      <c r="C35" t="s">
+        <v>276</v>
+      </c>
+      <c r="H35" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>221</v>
+      </c>
+      <c r="B36" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>223</v>
-      </c>
-      <c r="B33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C33" t="s">
-        <v>242</v>
-      </c>
-      <c r="D33" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>223</v>
-      </c>
-      <c r="B34" t="s">
-        <v>248</v>
-      </c>
-      <c r="C34" t="s">
-        <v>244</v>
-      </c>
-      <c r="D34" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>223</v>
-      </c>
-      <c r="B35" t="s">
-        <v>268</v>
-      </c>
-      <c r="C35" t="s">
-        <v>267</v>
-      </c>
-      <c r="D35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>223</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>221</v>
+      </c>
+      <c r="B37" t="s">
+        <v>217</v>
+      </c>
+      <c r="C37" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38" t="s">
+        <v>211</v>
+      </c>
+      <c r="D38" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" t="s">
+        <v>269</v>
+      </c>
+      <c r="C39" t="s">
         <v>270</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D39" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>221</v>
+      </c>
+      <c r="B40" t="s">
         <v>271</v>
       </c>
-      <c r="D36" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>223</v>
-      </c>
-      <c r="B37" t="s">
-        <v>269</v>
-      </c>
-      <c r="C37" t="s">
-        <v>266</v>
-      </c>
-      <c r="D37" t="s">
-        <v>257</v>
-      </c>
-      <c r="H37" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>247</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C40" t="s">
+        <v>272</v>
+      </c>
+      <c r="D40" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>221</v>
+      </c>
+      <c r="B41" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" t="s">
+        <v>243</v>
+      </c>
+      <c r="H41" t="s">
         <v>256</v>
       </c>
-      <c r="C38" t="s">
-        <v>238</v>
-      </c>
-      <c r="D38" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>247</v>
-      </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>221</v>
+      </c>
+      <c r="B42" t="s">
+        <v>228</v>
+      </c>
+      <c r="C42" t="s">
+        <v>209</v>
+      </c>
+      <c r="D42" t="s">
+        <v>243</v>
+      </c>
+      <c r="H42" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" t="s">
+        <v>261</v>
+      </c>
+      <c r="C43" t="s">
+        <v>262</v>
+      </c>
+      <c r="D43" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>220</v>
+      </c>
+      <c r="B44" t="s">
+        <v>292</v>
+      </c>
+      <c r="C44" t="s">
+        <v>212</v>
+      </c>
+      <c r="D44" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" t="s">
+        <v>293</v>
+      </c>
+      <c r="C45" t="s">
+        <v>186</v>
+      </c>
+      <c r="D45" t="s">
+        <v>243</v>
+      </c>
+      <c r="K45" t="s">
         <v>254</v>
       </c>
-      <c r="C39" t="s">
-        <v>239</v>
-      </c>
-      <c r="D39" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>220</v>
+      </c>
+      <c r="B46" t="s">
+        <v>294</v>
+      </c>
+      <c r="C46" t="s">
+        <v>207</v>
+      </c>
+      <c r="D46" t="s">
+        <v>243</v>
+      </c>
+      <c r="K46" t="s">
         <v>255</v>
       </c>
-      <c r="C40" t="s">
-        <v>240</v>
-      </c>
-      <c r="D40" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>247</v>
-      </c>
-      <c r="B41" t="s">
-        <v>262</v>
-      </c>
-      <c r="C41" t="s">
-        <v>263</v>
-      </c>
-      <c r="D41" t="s">
-        <v>261</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A1:K47">
+    <sortCondition ref="A1:A47"/>
+    <sortCondition ref="B1:B47"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="H28" r:id="rId1" xr:uid="{00B99229-3D0B-AA4C-B75B-579013D173A6}"/>
+    <hyperlink ref="H30" r:id="rId1" xr:uid="{00B99229-3D0B-AA4C-B75B-579013D173A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10732,49 +10999,49 @@
         <v>203</v>
       </c>
       <c r="G2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I2" t="s">
         <v>186</v>
       </c>
       <c r="J2" t="s">
+        <v>208</v>
+      </c>
+      <c r="K2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L2" t="s">
+        <v>235</v>
+      </c>
+      <c r="M2" t="s">
+        <v>236</v>
+      </c>
+      <c r="N2" t="s">
+        <v>237</v>
+      </c>
+      <c r="O2" t="s">
+        <v>238</v>
+      </c>
+      <c r="P2" t="s">
         <v>209</v>
       </c>
-      <c r="K2" t="s">
-        <v>237</v>
-      </c>
-      <c r="L2" t="s">
-        <v>238</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
+        <v>210</v>
+      </c>
+      <c r="R2" t="s">
         <v>239</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
         <v>240</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
         <v>241</v>
       </c>
-      <c r="P2" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>211</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>242</v>
-      </c>
-      <c r="S2" t="s">
-        <v>243</v>
-      </c>
-      <c r="T2" t="s">
-        <v>244</v>
-      </c>
-      <c r="U2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -10789,12 +11056,12 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
@@ -10804,62 +11071,62 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cognitive module updating other variables
</commit_message>
<xml_diff>
--- a/data-raw/BRFSS_SGM_CG_COG_States_2015-2017.xlsx
+++ b/data-raw/BRFSS_SGM_CG_COG_States_2015-2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Dropbox/BenAnalysis/BRFSS/brrfss/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcapistrant/Dropbox/BenAnalysis/BRFSS/brrfss/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9A0D64-ABAE-FF4C-9052-8E5A3200D92F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBCC195-ACFB-4C4A-B7BD-6F3D2A7F3D68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="21600" windowHeight="15940" activeTab="4" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
   </bookViews>
   <sheets>
     <sheet name="Module_States" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Covariates" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="415">
   <si>
     <t>Alabama</t>
   </si>
@@ -683,9 +683,6 @@
     <t>Veterans</t>
   </si>
   <si>
-    <t>Cognitive Fx</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -725,9 +722,6 @@
     <t>Marital Status</t>
   </si>
   <si>
-    <t>Number of Children</t>
-  </si>
-  <si>
     <t>Age, Imputed, 5 year categories</t>
   </si>
   <si>
@@ -779,9 +773,6 @@
     <t>Alcohol, Heavy Drinking</t>
   </si>
   <si>
-    <t>Race, imputed 5 level</t>
-  </si>
-  <si>
     <t>Race, multiple races</t>
   </si>
   <si>
@@ -800,9 +791,6 @@
     <t>Caregiving AJPH</t>
   </si>
   <si>
-    <t>CG AJPH paper dichotomized at 14+ days</t>
-  </si>
-  <si>
     <t>Chronic Diseases</t>
   </si>
   <si>
@@ -854,60 +842,12 @@
     <t>This is in an optional Module</t>
   </si>
   <si>
-    <t>https://bmcpublichealth.biomedcentral.com/articles/10.1186/1471-2458-12-685</t>
-  </si>
-  <si>
     <t>CG AJPH paper has Any of the Following(heart disease, stroke, diabetes, asthma, COPD, Arthritis, or non-skin cancer): CVDCRHD4, CVDSTRK3,DIABETE3,ASTHMA3,CHCOCNCR,CHCCOPD1,HAVARTH3. MCGUIRE et al JHNA 2010 had a count of conditions, too (asthma, arthritis,diabetes,heart disease)</t>
   </si>
   <si>
     <t>SEE NOTE</t>
   </si>
   <si>
-    <t>FRUIT2</t>
-  </si>
-  <si>
-    <t>Fruit Intake</t>
-  </si>
-  <si>
-    <t>Vegetable Intake</t>
-  </si>
-  <si>
-    <t>FVGREEN1 and VEGETAB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://bmcpublichealth.biomedcentral.com/articles/10.1186/1471-2458-12-685; FVGREEN, FVORANGE, VEGETAB1 in 2015 </t>
-  </si>
-  <si>
-    <t>Maybe only 2015/2017</t>
-  </si>
-  <si>
-    <t>EXERANY2</t>
-  </si>
-  <si>
-    <t>Phyiscal Activity - ever</t>
-  </si>
-  <si>
-    <t>Physical Activity - how often</t>
-  </si>
-  <si>
-    <t>Physical Activity - how long</t>
-  </si>
-  <si>
-    <t>EXEROFT1, EXEROFT2</t>
-  </si>
-  <si>
-    <t>EXERHMM1, EXERHMM2</t>
-  </si>
-  <si>
-    <t>Phyiscal Activity -strengthening</t>
-  </si>
-  <si>
-    <t>STRENGTH</t>
-  </si>
-  <si>
-    <t>Physical Activity is included in the odd years</t>
-  </si>
-  <si>
     <t>Employment Status</t>
   </si>
   <si>
@@ -986,14 +926,362 @@
     <t>agege65_d_fct</t>
   </si>
   <si>
-    <t xml:space="preserve">For </t>
+    <t>fem_d_num</t>
+  </si>
+  <si>
+    <t>0/1 (male/female)</t>
+  </si>
+  <si>
+    <t>Race/Ethnicity, imputed 5 level</t>
+  </si>
+  <si>
+    <t>Hispanic Ethnicity</t>
+  </si>
+  <si>
+    <t>X_HISPANC</t>
+  </si>
+  <si>
+    <t>The multiple race questionnaire does not capture ethnicity. If using this race variable, account for hispanic ethnicity separately.</t>
+  </si>
+  <si>
+    <t>ethn_cat_fct</t>
+  </si>
+  <si>
+    <t>race_cat_fct</t>
+  </si>
+  <si>
+    <t>mstat_cat_fct</t>
+  </si>
+  <si>
+    <t>chld_num</t>
+  </si>
+  <si>
+    <t>Number of Children in Household</t>
+  </si>
+  <si>
+    <t>chld_cat_fct</t>
+  </si>
+  <si>
+    <t>0-87</t>
+  </si>
+  <si>
+    <t>None, One, Two or More</t>
+  </si>
+  <si>
+    <t>X_CHLDCNT</t>
+  </si>
+  <si>
+    <t>Sex, Female</t>
+  </si>
+  <si>
+    <t>Age, Millennial</t>
+  </si>
+  <si>
+    <t>Age, 45+</t>
+  </si>
+  <si>
+    <t>Age, 65+</t>
+  </si>
+  <si>
+    <t>Married, Divorced, Widowed, Separated, Never Married, Coupled</t>
+  </si>
+  <si>
+    <t>vtrn_d_fct</t>
+  </si>
+  <si>
+    <t>vtrn_d_num</t>
+  </si>
+  <si>
+    <t>0/1 (Non-Vet/Veteran)</t>
+  </si>
+  <si>
+    <t>Non-Veteran, Veteran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       </t>
+  </si>
+  <si>
+    <t>White only, Black or African American only,  American Indian or Alaskan Native only,Asian only,  Native Hawaiian or other Pacific Islander only,Other race only,Multiracial</t>
+  </si>
+  <si>
+    <t>raceth_cat_fct</t>
+  </si>
+  <si>
+    <t>White Non-Hispanic; Black, Non-Hispanic;  Other, Non-Hispanic; Multiple, Non-Hispanic; Hispanic</t>
+  </si>
+  <si>
+    <t>Hispanic, Non-Hispanic</t>
+  </si>
+  <si>
+    <t>empl_cat_fct</t>
+  </si>
+  <si>
+    <t>Out of Work, Employed for wages, Self-Employed, A homemaker, A student, Retired, Unable to work</t>
+  </si>
+  <si>
+    <t>Refused set as NA</t>
+  </si>
+  <si>
+    <t>inc_cat_fct</t>
+  </si>
+  <si>
+    <t>educ_cat_fct</t>
+  </si>
+  <si>
+    <t>X_EDUCAG</t>
+  </si>
+  <si>
+    <t>&lt;High School, High School, Some College, College or More</t>
+  </si>
+  <si>
+    <t>Since DK/Refused is ~15%, these were kept in as one category ( 9, Don't know or refused)</t>
+  </si>
+  <si>
+    <t>&lt;$10,000, $10,000-$14,999,$15,000-19,999, $20,000-$24,999,$25,000-34,999, $35,000-$49,999,$50,000-74,999, $75,000+,Don't know or refused</t>
+  </si>
+  <si>
+    <t>drcost_d_fct</t>
+  </si>
+  <si>
+    <t>Variable reflects whether the respondent needed to see a doctor but could not because of cost. Yes responses reflcec economic insecurity regarding medical costs; No responses reflect no recent difficulty with medical costs.</t>
+  </si>
+  <si>
+    <t>hcplan_d_fct</t>
+  </si>
+  <si>
+    <t>chckup_cat_fct</t>
+  </si>
+  <si>
+    <t>&lt;1 year, 1-2 years, 2-5 years, 5+ years, Never</t>
+  </si>
+  <si>
+    <t>dntst_cat_fct</t>
+  </si>
+  <si>
+    <t>drnkbng_d_fct</t>
+  </si>
+  <si>
+    <t>drnkhvy_d_fct</t>
+  </si>
+  <si>
+    <t>bmi_cat_fct</t>
+  </si>
+  <si>
+    <t>Underweight, Normal Weight, Overweight, Obese, Unkown</t>
+  </si>
+  <si>
+    <t>~10% unknown, included as a category</t>
+  </si>
+  <si>
+    <t>smk_cat_fct</t>
+  </si>
+  <si>
+    <t>Current smoker, Former smoker, Never smoker</t>
+  </si>
+  <si>
+    <t>hiv_d_num</t>
+  </si>
+  <si>
+    <t>hiv_d_fct</t>
+  </si>
+  <si>
+    <t>DK/Refused set to NA</t>
+  </si>
+  <si>
+    <t>0/1 (No/Yes)</t>
+  </si>
+  <si>
+    <t>ltpa_d_fct</t>
+  </si>
+  <si>
+    <t>fluvac_date_num</t>
+  </si>
+  <si>
+    <t>fluvac_d_fct</t>
+  </si>
+  <si>
+    <t>fluvac_d_num</t>
+  </si>
+  <si>
+    <t>Used lubridate package to make date as useable</t>
+  </si>
+  <si>
+    <t>fluplc_cat_fct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doctor's office, Health dept, Health center, Community center, Store, Hospital, Emergency room, Workplace, Other, Canada/Mexico, School </t>
+  </si>
+  <si>
+    <t>12-20-15 - 12-20-16</t>
+  </si>
+  <si>
+    <t>numeric, date</t>
+  </si>
+  <si>
+    <t>srh_d_fct</t>
+  </si>
+  <si>
+    <t>srh_cat_fct</t>
+  </si>
+  <si>
+    <t>Good+, Fair/Poor</t>
+  </si>
+  <si>
+    <t>Excellent, Very Good, Good, Fair, Poor</t>
+  </si>
+  <si>
+    <t>lsat_d_fct</t>
+  </si>
+  <si>
+    <t>lsat_cat_fct</t>
+  </si>
+  <si>
+    <t>Very Satisfied, Satisfied, Dissatisfied, Very Dissatisfied</t>
+  </si>
+  <si>
+    <t>Satisfied/Dissatisfied</t>
+  </si>
+  <si>
+    <t>Dichotomized to reflect Satisfied &amp; Very satisfied vs. Dissatisfied &amp; Very Dissatisified</t>
+  </si>
+  <si>
+    <t>emsup_d_fct</t>
+  </si>
+  <si>
+    <t>emsup_cat_fct</t>
+  </si>
+  <si>
+    <t>Sometimes+, Rarely/Never</t>
+  </si>
+  <si>
+    <t>Always, Usually, Sometimes, Rarely, Never</t>
+  </si>
+  <si>
+    <t>Sometimes+ includes Sometimes, Usually, and Always</t>
+  </si>
+  <si>
+    <t>0-30</t>
+  </si>
+  <si>
+    <t>None (88) converted to 0</t>
+  </si>
+  <si>
+    <t>Yes: &gt;=14 days; No: 0-13 days; per CG AJPH paper</t>
+  </si>
+  <si>
+    <t>mentqol_num</t>
+  </si>
+  <si>
+    <t>mentqol14_d_fct</t>
+  </si>
+  <si>
+    <t>physqol_num</t>
+  </si>
+  <si>
+    <t>physqol14_d_fct</t>
+  </si>
+  <si>
+    <t>dep_d_fct</t>
+  </si>
+  <si>
+    <t>chron_num</t>
+  </si>
+  <si>
+    <t>chron_d_fct</t>
+  </si>
+  <si>
+    <t>0-7</t>
+  </si>
+  <si>
+    <t>Cognitive Fx - Memory Loss / Confusion</t>
+  </si>
+  <si>
+    <t>Cognitive Fx - Difficulty with Household Tasks</t>
+  </si>
+  <si>
+    <t>memloss_d_num</t>
+  </si>
+  <si>
+    <t>memloss_d_fct</t>
+  </si>
+  <si>
+    <t>memhous_cat_fct</t>
+  </si>
+  <si>
+    <t>memhous_d_fct</t>
+  </si>
+  <si>
+    <t>Chronic Diseases - Heart Disease</t>
+  </si>
+  <si>
+    <t>Chronic Diseases - Stroke</t>
+  </si>
+  <si>
+    <t>Chronic Diseases - Diabetes</t>
+  </si>
+  <si>
+    <t>Chronic Diseases - Asthma</t>
+  </si>
+  <si>
+    <t>Chronic Diseases - COPD</t>
+  </si>
+  <si>
+    <t>Chronic Diseases - Cancer</t>
+  </si>
+  <si>
+    <t>CVDCRHD4</t>
+  </si>
+  <si>
+    <t>CVDSTRK3</t>
+  </si>
+  <si>
+    <t>DIABETE3</t>
+  </si>
+  <si>
+    <t>ASTHMA3</t>
+  </si>
+  <si>
+    <t>CHCOCNCR</t>
+  </si>
+  <si>
+    <t>CHCCOPD1</t>
+  </si>
+  <si>
+    <t>Chronic Diseases - Arthritis</t>
+  </si>
+  <si>
+    <t>HAVARTH3</t>
+  </si>
+  <si>
+    <t>cvd_d_num</t>
+  </si>
+  <si>
+    <t>strk_d_num</t>
+  </si>
+  <si>
+    <t>diab_d_num</t>
+  </si>
+  <si>
+    <t>asth_d_num</t>
+  </si>
+  <si>
+    <t>cncr_d_num</t>
+  </si>
+  <si>
+    <t>copd_d_num</t>
+  </si>
+  <si>
+    <t>arth_d_num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1040,14 +1328,6 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1066,11 +1346,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1081,11 +1360,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -10110,10 +10389,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FC520E-C64D-6242-ADD9-027A4DCE44BD}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10127,7 +10407,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>215</v>
@@ -10153,10 +10433,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C2" t="s">
         <v>206</v>
@@ -10165,24 +10445,24 @@
         <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="F2" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="G2" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="H2" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
         <v>206</v>
@@ -10191,76 +10471,76 @@
         <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="F3" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="G3" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="H3" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>314</v>
       </c>
       <c r="C4" t="s">
         <v>206</v>
       </c>
       <c r="D4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E4" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="F4" t="s">
-        <v>306</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>307</v>
+        <v>286</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>287</v>
       </c>
       <c r="H4" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>314</v>
       </c>
       <c r="C5" t="s">
         <v>206</v>
       </c>
       <c r="D5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E5" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="F5" t="s">
-        <v>303</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>309</v>
+        <v>283</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>289</v>
       </c>
       <c r="H5" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s">
-        <v>232</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s">
         <v>206</v>
@@ -10269,24 +10549,24 @@
         <v>200</v>
       </c>
       <c r="E6" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="F6" t="s">
-        <v>306</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>307</v>
+        <v>286</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>287</v>
       </c>
       <c r="H6" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
-        <v>232</v>
+        <v>315</v>
       </c>
       <c r="C7" t="s">
         <v>206</v>
@@ -10295,617 +10575,1369 @@
         <v>200</v>
       </c>
       <c r="E7" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="F7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>309</v>
+        <v>283</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>289</v>
       </c>
       <c r="H7" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>316</v>
       </c>
       <c r="C8" t="s">
         <v>206</v>
       </c>
       <c r="D8" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="E8" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="F8" t="s">
-        <v>306</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>307</v>
+        <v>286</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>287</v>
       </c>
       <c r="H8" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>316</v>
       </c>
       <c r="C9" t="s">
         <v>206</v>
       </c>
       <c r="D9" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="E9" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="F9" t="s">
-        <v>303</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>309</v>
+        <v>283</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>289</v>
       </c>
       <c r="H9" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
         <v>208</v>
       </c>
       <c r="D10" t="s">
-        <v>243</v>
+        <v>241</v>
+      </c>
+      <c r="E10" t="s">
+        <v>306</v>
+      </c>
+      <c r="F10" t="s">
+        <v>279</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>241</v>
+      </c>
+      <c r="E11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F11" t="s">
+        <v>279</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>308</v>
       </c>
       <c r="C12" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>246</v>
+        <v>200</v>
+      </c>
+      <c r="E12" t="s">
+        <v>307</v>
+      </c>
+      <c r="F12" t="s">
+        <v>277</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>308</v>
       </c>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>312</v>
       </c>
       <c r="D13" t="s">
-        <v>200</v>
+        <v>241</v>
+      </c>
+      <c r="E13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F13" t="s">
+        <v>279</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>229</v>
+        <v>300</v>
       </c>
       <c r="C14" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="D14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E14" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="F14" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="G14" t="s">
-        <v>304</v>
-      </c>
-      <c r="H14" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>301</v>
       </c>
       <c r="C15" t="s">
-        <v>177</v>
+        <v>302</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
+        <v>241</v>
+      </c>
+      <c r="E15" t="s">
+        <v>304</v>
+      </c>
+      <c r="F15" t="s">
+        <v>279</v>
+      </c>
+      <c r="G15" t="s">
+        <v>327</v>
+      </c>
+      <c r="H15" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B16" t="s">
         <v>247</v>
       </c>
       <c r="C16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D16" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>325</v>
+      </c>
+      <c r="F16" t="s">
+        <v>279</v>
+      </c>
+      <c r="G16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E17" t="s">
+        <v>282</v>
+      </c>
+      <c r="F17" t="s">
+        <v>283</v>
+      </c>
+      <c r="G17" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" t="s">
+        <v>313</v>
+      </c>
+      <c r="C18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D18" t="s">
+        <v>241</v>
+      </c>
+      <c r="E18" t="s">
+        <v>298</v>
+      </c>
+      <c r="F18" t="s">
+        <v>286</v>
+      </c>
+      <c r="G18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E19" t="s">
+        <v>319</v>
+      </c>
+      <c r="F19" t="s">
+        <v>286</v>
+      </c>
+      <c r="G19" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" t="s">
+        <v>200</v>
+      </c>
+      <c r="E20" t="s">
+        <v>318</v>
+      </c>
+      <c r="F20" t="s">
+        <v>283</v>
+      </c>
+      <c r="G20" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" t="s">
+        <v>245</v>
+      </c>
+      <c r="C21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" t="s">
+        <v>343</v>
+      </c>
+      <c r="F21" t="s">
+        <v>283</v>
+      </c>
+      <c r="G21" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C22" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" t="s">
+        <v>244</v>
+      </c>
+      <c r="E22" t="s">
+        <v>344</v>
+      </c>
+      <c r="F22" t="s">
+        <v>283</v>
+      </c>
+      <c r="G22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" t="s">
+        <v>241</v>
+      </c>
+      <c r="E23" t="s">
+        <v>345</v>
+      </c>
+      <c r="F23" t="s">
+        <v>279</v>
+      </c>
+      <c r="G23" t="s">
+        <v>346</v>
+      </c>
+      <c r="H23" t="s">
+        <v>347</v>
+      </c>
+      <c r="K23" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" t="s">
+        <v>243</v>
+      </c>
+      <c r="C24" t="s">
+        <v>239</v>
+      </c>
+      <c r="D24" t="s">
+        <v>244</v>
+      </c>
+      <c r="E24" t="s">
+        <v>350</v>
+      </c>
+      <c r="F24" t="s">
+        <v>286</v>
+      </c>
+      <c r="G24" t="s">
+        <v>353</v>
+      </c>
+      <c r="H24" t="s">
+        <v>352</v>
+      </c>
+      <c r="K24" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>221</v>
+      </c>
+      <c r="B25" t="s">
+        <v>243</v>
+      </c>
+      <c r="C25" t="s">
+        <v>239</v>
+      </c>
+      <c r="D25" t="s">
+        <v>244</v>
+      </c>
+      <c r="E25" t="s">
+        <v>351</v>
+      </c>
+      <c r="F25" t="s">
+        <v>283</v>
+      </c>
+      <c r="G25" t="s">
+        <v>289</v>
+      </c>
+      <c r="H25" t="s">
+        <v>352</v>
+      </c>
+      <c r="K25" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>221</v>
+      </c>
+      <c r="B26" t="s">
+        <v>261</v>
+      </c>
+      <c r="C26" t="s">
+        <v>260</v>
+      </c>
+      <c r="D26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E26" t="s">
+        <v>356</v>
+      </c>
+      <c r="F26" t="s">
+        <v>283</v>
+      </c>
+      <c r="G26" t="s">
+        <v>289</v>
+      </c>
+      <c r="H26" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>221</v>
+      </c>
+      <c r="B27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C27" t="s">
+        <v>260</v>
+      </c>
+      <c r="D27" t="s">
+        <v>251</v>
+      </c>
+      <c r="E27" t="s">
+        <v>357</v>
+      </c>
+      <c r="F27" t="s">
+        <v>286</v>
+      </c>
+      <c r="G27" t="s">
+        <v>353</v>
+      </c>
+      <c r="H27" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B28" t="s">
+        <v>263</v>
+      </c>
+      <c r="C28" t="s">
+        <v>264</v>
+      </c>
+      <c r="D28" t="s">
+        <v>251</v>
+      </c>
+      <c r="E28" t="s">
+        <v>355</v>
+      </c>
+      <c r="F28" t="s">
+        <v>362</v>
+      </c>
+      <c r="G28" t="s">
+        <v>361</v>
+      </c>
+      <c r="H28" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>221</v>
+      </c>
+      <c r="B29" t="s">
+        <v>262</v>
+      </c>
+      <c r="C29" t="s">
+        <v>259</v>
+      </c>
+      <c r="D29" t="s">
+        <v>251</v>
+      </c>
+      <c r="E29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G29" t="s">
+        <v>360</v>
+      </c>
+      <c r="H29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" t="s">
         <v>222</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C30" t="s">
+        <v>214</v>
+      </c>
+      <c r="D30" t="s">
+        <v>200</v>
+      </c>
+      <c r="E30" t="s">
+        <v>354</v>
+      </c>
+      <c r="F30" t="s">
+        <v>283</v>
+      </c>
+      <c r="G30" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" t="s">
+        <v>213</v>
+      </c>
+      <c r="D31" t="s">
+        <v>241</v>
+      </c>
+      <c r="E31" t="s">
+        <v>348</v>
+      </c>
+      <c r="F31" t="s">
+        <v>279</v>
+      </c>
+      <c r="G31" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>242</v>
+      </c>
+      <c r="B32" t="s">
         <v>248</v>
       </c>
-      <c r="C17" t="s">
-        <v>239</v>
-      </c>
-      <c r="D17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>222</v>
-      </c>
-      <c r="B18" t="s">
-        <v>224</v>
-      </c>
-      <c r="C18" t="s">
-        <v>195</v>
-      </c>
-      <c r="D18" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>222</v>
-      </c>
-      <c r="B19" t="s">
-        <v>278</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C32" t="s">
+        <v>234</v>
+      </c>
+      <c r="D32" t="s">
+        <v>244</v>
+      </c>
+      <c r="E32" t="s">
+        <v>337</v>
+      </c>
+      <c r="F32" t="s">
+        <v>283</v>
+      </c>
+      <c r="G32" t="s">
+        <v>289</v>
+      </c>
+      <c r="H32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>242</v>
+      </c>
+      <c r="B33" t="s">
+        <v>250</v>
+      </c>
+      <c r="C33" t="s">
+        <v>233</v>
+      </c>
+      <c r="D33" t="s">
+        <v>244</v>
+      </c>
+      <c r="E33" t="s">
+        <v>339</v>
+      </c>
+      <c r="F33" t="s">
+        <v>283</v>
+      </c>
+      <c r="G33" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B34" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34" t="s">
+        <v>235</v>
+      </c>
+      <c r="D34" t="s">
+        <v>244</v>
+      </c>
+      <c r="E34" t="s">
+        <v>340</v>
+      </c>
+      <c r="F34" t="s">
+        <v>279</v>
+      </c>
+      <c r="G34" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>242</v>
+      </c>
+      <c r="B35" t="s">
+        <v>255</v>
+      </c>
+      <c r="C35" t="s">
+        <v>256</v>
+      </c>
+      <c r="D35" t="s">
+        <v>254</v>
+      </c>
+      <c r="E35" t="s">
+        <v>342</v>
+      </c>
+      <c r="F35" t="s">
+        <v>279</v>
+      </c>
+      <c r="G35" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>220</v>
+      </c>
+      <c r="B36" t="s">
+        <v>253</v>
+      </c>
+      <c r="C36" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" t="s">
+        <v>241</v>
+      </c>
+      <c r="E36" t="s">
+        <v>385</v>
+      </c>
+      <c r="F36" t="s">
         <v>277</v>
       </c>
-      <c r="H19" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>222</v>
-      </c>
-      <c r="B20" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="G36" t="s">
+        <v>387</v>
+      </c>
+      <c r="H36" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" t="s">
+        <v>253</v>
+      </c>
+      <c r="C37" t="s">
+        <v>271</v>
+      </c>
+      <c r="D37" t="s">
         <v>241</v>
       </c>
-      <c r="D20" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>222</v>
-      </c>
-      <c r="B21" t="s">
-        <v>265</v>
-      </c>
-      <c r="C21" t="s">
-        <v>264</v>
-      </c>
-      <c r="D21" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>222</v>
-      </c>
-      <c r="B22" t="s">
-        <v>267</v>
-      </c>
-      <c r="C22" t="s">
-        <v>268</v>
-      </c>
-      <c r="D22" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>222</v>
-      </c>
-      <c r="B23" t="s">
-        <v>266</v>
-      </c>
-      <c r="C23" t="s">
-        <v>263</v>
-      </c>
-      <c r="D23" t="s">
-        <v>254</v>
-      </c>
-      <c r="H23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>222</v>
-      </c>
-      <c r="B24" t="s">
-        <v>223</v>
-      </c>
-      <c r="C24" t="s">
-        <v>214</v>
-      </c>
-      <c r="D24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>222</v>
-      </c>
-      <c r="B25" t="s">
-        <v>284</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E37" t="s">
+        <v>386</v>
+      </c>
+      <c r="F37" t="s">
         <v>283</v>
       </c>
-      <c r="H25" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="G37" t="s">
         <v>289</v>
       </c>
-      <c r="C26" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>222</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="H37" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>220</v>
+      </c>
+      <c r="B38" t="s">
+        <v>394</v>
+      </c>
+      <c r="C38" t="s">
+        <v>400</v>
+      </c>
+      <c r="D38" t="s">
+        <v>241</v>
+      </c>
+      <c r="E38" t="s">
+        <v>408</v>
+      </c>
+      <c r="F38" t="s">
         <v>286</v>
       </c>
-      <c r="C27" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>222</v>
-      </c>
-      <c r="B28" t="s">
-        <v>285</v>
-      </c>
-      <c r="C28" t="s">
-        <v>287</v>
-      </c>
-      <c r="H28" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>222</v>
-      </c>
-      <c r="B29" t="s">
-        <v>225</v>
-      </c>
-      <c r="C29" t="s">
-        <v>213</v>
-      </c>
-      <c r="D29" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>222</v>
-      </c>
-      <c r="B30" t="s">
-        <v>279</v>
-      </c>
-      <c r="C30" t="s">
-        <v>280</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>244</v>
-      </c>
-      <c r="B31" t="s">
-        <v>251</v>
-      </c>
-      <c r="C31" t="s">
-        <v>236</v>
-      </c>
-      <c r="D31" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B32" t="s">
-        <v>253</v>
-      </c>
-      <c r="C32" t="s">
-        <v>235</v>
-      </c>
-      <c r="D32" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B33" t="s">
-        <v>252</v>
-      </c>
-      <c r="C33" t="s">
-        <v>237</v>
-      </c>
-      <c r="D33" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>244</v>
-      </c>
-      <c r="B34" t="s">
-        <v>259</v>
-      </c>
-      <c r="C34" t="s">
-        <v>260</v>
-      </c>
-      <c r="D34" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>221</v>
-      </c>
-      <c r="B35" t="s">
-        <v>257</v>
-      </c>
-      <c r="C35" t="s">
-        <v>276</v>
-      </c>
-      <c r="H35" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>221</v>
-      </c>
-      <c r="B36" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" t="s">
-        <v>201</v>
-      </c>
-      <c r="D36" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>221</v>
-      </c>
-      <c r="B37" t="s">
-        <v>217</v>
-      </c>
-      <c r="C37" t="s">
-        <v>202</v>
-      </c>
-      <c r="D37" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>221</v>
-      </c>
-      <c r="B38" t="s">
-        <v>226</v>
-      </c>
-      <c r="C38" t="s">
-        <v>211</v>
-      </c>
-      <c r="D38" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B39" t="s">
-        <v>269</v>
+        <v>395</v>
       </c>
       <c r="C39" t="s">
-        <v>270</v>
+        <v>401</v>
       </c>
       <c r="D39" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="E39" t="s">
+        <v>409</v>
+      </c>
+      <c r="F39" t="s">
+        <v>286</v>
+      </c>
+      <c r="G39" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B40" t="s">
-        <v>271</v>
+        <v>396</v>
       </c>
       <c r="C40" t="s">
-        <v>272</v>
+        <v>402</v>
       </c>
       <c r="D40" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="E40" t="s">
+        <v>410</v>
+      </c>
+      <c r="F40" t="s">
+        <v>286</v>
+      </c>
+      <c r="G40" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B41" t="s">
-        <v>227</v>
+        <v>397</v>
       </c>
       <c r="C41" t="s">
-        <v>210</v>
+        <v>403</v>
       </c>
       <c r="D41" t="s">
-        <v>243</v>
-      </c>
-      <c r="H41" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="E41" t="s">
+        <v>411</v>
+      </c>
+      <c r="F41" t="s">
+        <v>286</v>
+      </c>
+      <c r="G41" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B42" t="s">
-        <v>228</v>
+        <v>406</v>
       </c>
       <c r="C42" t="s">
-        <v>209</v>
+        <v>407</v>
       </c>
       <c r="D42" t="s">
-        <v>243</v>
-      </c>
-      <c r="H42" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="E42" t="s">
+        <v>414</v>
+      </c>
+      <c r="F42" t="s">
+        <v>286</v>
+      </c>
+      <c r="G42" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B43" t="s">
-        <v>261</v>
+        <v>398</v>
       </c>
       <c r="C43" t="s">
-        <v>262</v>
+        <v>405</v>
       </c>
       <c r="D43" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="E43" t="s">
+        <v>413</v>
+      </c>
+      <c r="F43" t="s">
+        <v>286</v>
+      </c>
+      <c r="G43" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>220</v>
       </c>
       <c r="B44" t="s">
-        <v>292</v>
+        <v>399</v>
       </c>
       <c r="C44" t="s">
-        <v>212</v>
+        <v>404</v>
       </c>
       <c r="D44" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="E44" t="s">
+        <v>412</v>
+      </c>
+      <c r="F44" t="s">
+        <v>286</v>
+      </c>
+      <c r="G44" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>220</v>
       </c>
       <c r="B45" t="s">
-        <v>293</v>
+        <v>388</v>
       </c>
       <c r="C45" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="D45" t="s">
-        <v>243</v>
-      </c>
-      <c r="K45" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+      <c r="E45" t="s">
+        <v>390</v>
+      </c>
+      <c r="F45" t="s">
+        <v>286</v>
+      </c>
+      <c r="G45" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>220</v>
       </c>
       <c r="B46" t="s">
-        <v>294</v>
+        <v>388</v>
       </c>
       <c r="C46" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D46" t="s">
-        <v>243</v>
-      </c>
-      <c r="K46" t="s">
-        <v>255</v>
+        <v>200</v>
+      </c>
+      <c r="E46" t="s">
+        <v>391</v>
+      </c>
+      <c r="F46" t="s">
+        <v>283</v>
+      </c>
+      <c r="G46" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>220</v>
+      </c>
+      <c r="B47" t="s">
+        <v>389</v>
+      </c>
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" t="s">
+        <v>200</v>
+      </c>
+      <c r="E47" t="s">
+        <v>392</v>
+      </c>
+      <c r="F47" t="s">
+        <v>279</v>
+      </c>
+      <c r="G47" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" t="s">
+        <v>389</v>
+      </c>
+      <c r="C48" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" t="s">
+        <v>393</v>
+      </c>
+      <c r="F48" t="s">
+        <v>283</v>
+      </c>
+      <c r="G48" t="s">
+        <v>374</v>
+      </c>
+      <c r="H48" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B49" t="s">
+        <v>225</v>
+      </c>
+      <c r="C49" t="s">
+        <v>211</v>
+      </c>
+      <c r="D49" t="s">
+        <v>200</v>
+      </c>
+      <c r="E49" t="s">
+        <v>384</v>
+      </c>
+      <c r="F49" t="s">
+        <v>283</v>
+      </c>
+      <c r="G49" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B50" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50" t="s">
+        <v>266</v>
+      </c>
+      <c r="D50" t="s">
+        <v>254</v>
+      </c>
+      <c r="E50" t="s">
+        <v>372</v>
+      </c>
+      <c r="F50" t="s">
+        <v>283</v>
+      </c>
+      <c r="G50" t="s">
+        <v>374</v>
+      </c>
+      <c r="H50" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" t="s">
+        <v>265</v>
+      </c>
+      <c r="C51" t="s">
+        <v>266</v>
+      </c>
+      <c r="D51" t="s">
+        <v>254</v>
+      </c>
+      <c r="E51" t="s">
+        <v>373</v>
+      </c>
+      <c r="F51" t="s">
+        <v>279</v>
+      </c>
+      <c r="G51" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" t="s">
+        <v>267</v>
+      </c>
+      <c r="C52" t="s">
+        <v>268</v>
+      </c>
+      <c r="D52" t="s">
+        <v>254</v>
+      </c>
+      <c r="E52" t="s">
+        <v>367</v>
+      </c>
+      <c r="F52" t="s">
+        <v>283</v>
+      </c>
+      <c r="G52" t="s">
+        <v>370</v>
+      </c>
+      <c r="H52" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>220</v>
+      </c>
+      <c r="B53" t="s">
+        <v>267</v>
+      </c>
+      <c r="C53" t="s">
+        <v>268</v>
+      </c>
+      <c r="D53" t="s">
+        <v>254</v>
+      </c>
+      <c r="E53" t="s">
+        <v>368</v>
+      </c>
+      <c r="F53" t="s">
+        <v>283</v>
+      </c>
+      <c r="G53" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>220</v>
+      </c>
+      <c r="B54" t="s">
+        <v>226</v>
+      </c>
+      <c r="C54" t="s">
+        <v>210</v>
+      </c>
+      <c r="D54" t="s">
+        <v>241</v>
+      </c>
+      <c r="E54" t="s">
+        <v>380</v>
+      </c>
+      <c r="F54" t="s">
+        <v>277</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H54" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>220</v>
+      </c>
+      <c r="B55" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" t="s">
+        <v>210</v>
+      </c>
+      <c r="D55" t="s">
+        <v>241</v>
+      </c>
+      <c r="E55" t="s">
+        <v>381</v>
+      </c>
+      <c r="F55" t="s">
+        <v>283</v>
+      </c>
+      <c r="G55" t="s">
+        <v>289</v>
+      </c>
+      <c r="H55" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>220</v>
+      </c>
+      <c r="B56" t="s">
+        <v>227</v>
+      </c>
+      <c r="C56" t="s">
+        <v>209</v>
+      </c>
+      <c r="D56" t="s">
+        <v>241</v>
+      </c>
+      <c r="E56" t="s">
+        <v>382</v>
+      </c>
+      <c r="F56" t="s">
+        <v>277</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H56" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>220</v>
+      </c>
+      <c r="B57" t="s">
+        <v>227</v>
+      </c>
+      <c r="C57" t="s">
+        <v>209</v>
+      </c>
+      <c r="D57" t="s">
+        <v>241</v>
+      </c>
+      <c r="E57" t="s">
+        <v>383</v>
+      </c>
+      <c r="F57" t="s">
+        <v>283</v>
+      </c>
+      <c r="G57" t="s">
+        <v>289</v>
+      </c>
+      <c r="H57" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>220</v>
+      </c>
+      <c r="B58" t="s">
+        <v>257</v>
+      </c>
+      <c r="C58" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" t="s">
+        <v>254</v>
+      </c>
+      <c r="E58" t="s">
+        <v>363</v>
+      </c>
+      <c r="F58" t="s">
+        <v>283</v>
+      </c>
+      <c r="G58" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59" t="s">
+        <v>257</v>
+      </c>
+      <c r="C59" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" t="s">
+        <v>254</v>
+      </c>
+      <c r="E59" t="s">
+        <v>364</v>
+      </c>
+      <c r="F59" t="s">
+        <v>279</v>
+      </c>
+      <c r="G59" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>219</v>
+      </c>
+      <c r="B60" t="s">
+        <v>272</v>
+      </c>
+      <c r="C60" t="s">
+        <v>212</v>
+      </c>
+      <c r="D60" t="s">
+        <v>200</v>
+      </c>
+      <c r="E60" t="s">
+        <v>328</v>
+      </c>
+      <c r="F60" t="s">
+        <v>279</v>
+      </c>
+      <c r="G60" t="s">
+        <v>329</v>
+      </c>
+      <c r="H60" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>219</v>
+      </c>
+      <c r="B61" t="s">
+        <v>273</v>
+      </c>
+      <c r="C61" t="s">
+        <v>186</v>
+      </c>
+      <c r="D61" t="s">
+        <v>241</v>
+      </c>
+      <c r="E61" t="s">
+        <v>331</v>
+      </c>
+      <c r="F61" t="s">
+        <v>279</v>
+      </c>
+      <c r="G61" t="s">
+        <v>336</v>
+      </c>
+      <c r="H61" t="s">
+        <v>335</v>
+      </c>
+      <c r="K61" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>219</v>
+      </c>
+      <c r="B62" t="s">
+        <v>274</v>
+      </c>
+      <c r="C62" t="s">
+        <v>333</v>
+      </c>
+      <c r="D62" t="s">
+        <v>241</v>
+      </c>
+      <c r="E62" t="s">
+        <v>332</v>
+      </c>
+      <c r="F62" t="s">
+        <v>279</v>
+      </c>
+      <c r="G62" t="s">
+        <v>334</v>
+      </c>
+      <c r="H62" t="s">
+        <v>330</v>
+      </c>
+      <c r="K62" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:K47">
-    <sortCondition ref="A1:A47"/>
-    <sortCondition ref="B1:B47"/>
+  <sortState ref="A1:K63">
+    <sortCondition ref="A1:A63"/>
+    <sortCondition ref="B1:B63"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="H30" r:id="rId1" xr:uid="{00B99229-3D0B-AA4C-B75B-579013D173A6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10999,7 +12031,7 @@
         <v>203</v>
       </c>
       <c r="G2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H2" t="s">
         <v>207</v>
@@ -11011,19 +12043,19 @@
         <v>208</v>
       </c>
       <c r="K2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L2" t="s">
+        <v>233</v>
+      </c>
+      <c r="M2" t="s">
         <v>234</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>235</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>236</v>
-      </c>
-      <c r="N2" t="s">
-        <v>237</v>
-      </c>
-      <c r="O2" t="s">
-        <v>238</v>
       </c>
       <c r="P2" t="s">
         <v>209</v>
@@ -11032,16 +12064,16 @@
         <v>210</v>
       </c>
       <c r="R2" t="s">
+        <v>237</v>
+      </c>
+      <c r="S2" t="s">
+        <v>238</v>
+      </c>
+      <c r="T2" t="s">
         <v>239</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>240</v>
-      </c>
-      <c r="T2" t="s">
-        <v>241</v>
-      </c>
-      <c r="U2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -11056,7 +12088,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -11076,27 +12108,27 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -11111,22 +12143,22 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing names from brrfss to brfss, renaming package (brfssR)
</commit_message>
<xml_diff>
--- a/data-raw/BRFSS_SGM_CG_COG_States_2015-2017.xlsx
+++ b/data-raw/BRFSS_SGM_CG_COG_States_2015-2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcapistrant/Dropbox/BenAnalysis/BRFSS/brrfss/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Dropbox/BenAnalysis/BRFSS/brfssR/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40ED228-CDAA-3249-B754-6FCFA740B549}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F5EE0CA-300C-E048-9273-6B18CFC305BE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="18000" firstSheet="1" activeTab="6" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="8" xr2:uid="{1EA68701-B437-4F46-81E0-6C2E6881A539}"/>
   </bookViews>
   <sheets>
     <sheet name="Module_States" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId3"/>
     <sheet name="CG_States" sheetId="4" r:id="rId4"/>
     <sheet name="COG_States" sheetId="5" r:id="rId5"/>
-    <sheet name="Covariates" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId7"/>
+    <sheet name="EMSPT_States" sheetId="9" r:id="rId6"/>
+    <sheet name="Covariates" sheetId="6" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId8"/>
+    <sheet name="Cog_Covariates" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="459">
   <si>
     <t>Alabama</t>
   </si>
@@ -1339,10 +1340,70 @@
     <t>2016-2017</t>
   </si>
   <si>
+    <t>EMSPT2015</t>
+  </si>
+  <si>
+    <t>EMSPT2015_Version</t>
+  </si>
+  <si>
+    <t>EMSPT2015_Weight</t>
+  </si>
+  <si>
+    <t>EMSPT2016</t>
+  </si>
+  <si>
+    <t>EMSPT2016_Version</t>
+  </si>
+  <si>
+    <t>EMSPT2016_Weight</t>
+  </si>
+  <si>
+    <t>EMSPT2017</t>
+  </si>
+  <si>
+    <t>EMSPT2017_Version</t>
+  </si>
+  <si>
+    <t>EMSPT2017_Weight</t>
+  </si>
+  <si>
+    <t>EMSPTNumber</t>
+  </si>
+  <si>
+    <t>EMSPTAny</t>
+  </si>
+  <si>
+    <t>_LLCPWT</t>
+  </si>
+  <si>
+    <t>_LCPWTV1</t>
+  </si>
+  <si>
+    <t>_LCPWTV2</t>
+  </si>
+  <si>
+    <t>EMSPT2014</t>
+  </si>
+  <si>
+    <t>EMSPT2014_Version</t>
+  </si>
+  <si>
+    <t>EMSPT2014_Weight</t>
+  </si>
+  <si>
+    <t>Cognitive Function</t>
+  </si>
+  <si>
+    <t>CIMEMLOS: During the past 12 months, have you experienced confusion or memory loss that is happening more often or is getting worse? 0/1 (No/Yes)</t>
+  </si>
+  <si>
+    <t>CIMEMLOS: During the past 12 months, have you experienced confusion or memory loss that is happening more often or is getting worse? No/Yes</t>
+  </si>
+  <si>
+    <t>CDHOUSE: During the past 12 months, as a result of confusion or memory loss, how often have you given up day-to-day household activities or chores you used to do, such as cooking, cleaning, taking medications, driving, or paying bills? Always, Usually, Sometimes, Rarely, Never</t>
+  </si>
+  <si>
     <t>Always, Usually, Sometimes, Rarely, Never, or Never Needs (This keeps in those who didn't need help rather than setting them to missing in cog_help_cat_fct)</t>
-  </si>
-  <si>
-    <t>Cognitive Function</t>
   </si>
   <si>
     <t>During the past 12 months, how often has confusion or memory loss interfered with your ability
@@ -1351,15 +1412,6 @@
   <si>
     <t>During the past 12 months, how often has confusion or memory loss interfered with your ability
 to work, volunteer, or engage in social activities outside the home? Always, Usually, Sometimes, Rarely, Never, or Never Needs (This keeps in those who didn't need help rather than setting them to missing in cog_social_cat_fct)</t>
-  </si>
-  <si>
-    <t>CIMEMLOS: During the past 12 months, have you experienced confusion or memory loss that is happening more often or is getting worse? 0/1 (No/Yes)</t>
-  </si>
-  <si>
-    <t>CIMEMLOS: During the past 12 months, have you experienced confusion or memory loss that is happening more often or is getting worse? No/Yes</t>
-  </si>
-  <si>
-    <t>CDHOUSE: During the past 12 months, as a result of confusion or memory loss, how often have you given up day-to-day household activities or chores you used to do, such as cooking, cleaning, taking medications, driving, or paying bills? Always, Usually, Sometimes, Rarely, Never</t>
   </si>
 </sst>
 </file>
@@ -4263,7 +4315,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U52" sqref="U52"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6982,7 +7034,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8947,7 +8999,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10851,12 +10903,2088 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F85786-3474-114E-AD51-ED1C4978AD6C}">
+  <dimension ref="A1:Q55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="5.5" style="3"/>
+    <col min="3" max="3" width="14.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.83203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="5.5" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <f t="shared" ref="P2:P33" si="0">SUM(G2:M2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>IF(OR(G2=1,J2=1,M2=1),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" ref="Q3:Q54" si="1">IF(OR(G3=1,J3=1,M3=1),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="P4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="P5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="P6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A7" s="3">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="P7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A10" s="3">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="P10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A12" s="3">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="P12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A13" s="3">
+        <v>66</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="P13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="P14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A16" s="3">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A17" s="3">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4"/>
+      <c r="P17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A18" s="3">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="P18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A19" s="3">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
+        <v>21</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A21" s="3">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
+        <v>23</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A23" s="3">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A24" s="3">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="3">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A25" s="3">
+        <v>26</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="P25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A26" s="3">
+        <v>27</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="M26" s="3">
+        <v>1</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="P26" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Q26" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A27" s="3">
+        <v>28</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="M27" s="3">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4"/>
+      <c r="P27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A28" s="3">
+        <v>29</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A29" s="3">
+        <v>30</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A30" s="3">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0</v>
+      </c>
+      <c r="P30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A31" s="3">
+        <v>32</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4"/>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4"/>
+      <c r="M31" s="3">
+        <v>0</v>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="P31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A32" s="3">
+        <v>33</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A33" s="3">
+        <v>34</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A34" s="3">
+        <v>35</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="3">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="3">
+        <f t="shared" ref="P34:P54" si="2">SUM(G34:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A35" s="3">
+        <v>36</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A36" s="3">
+        <v>37</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="3">
+        <v>0</v>
+      </c>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A37" s="3">
+        <v>38</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4"/>
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+      <c r="N37" s="4"/>
+      <c r="P37" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A38" s="3">
+        <v>39</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="4"/>
+      <c r="M38" s="3">
+        <v>1</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="P38" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q38" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
+        <v>40</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="G39" s="3">
+        <v>1</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0</v>
+      </c>
+      <c r="M39" s="3">
+        <v>0</v>
+      </c>
+      <c r="P39" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q39" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
+        <v>41</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="3">
+        <v>0</v>
+      </c>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="3">
+        <v>0</v>
+      </c>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A41" s="3">
+        <v>42</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4"/>
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4"/>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+      <c r="N41" s="4"/>
+      <c r="P41" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A42" s="3">
+        <v>72</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4"/>
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4"/>
+      <c r="M42" s="3">
+        <v>0</v>
+      </c>
+      <c r="N42" s="4"/>
+      <c r="P42" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A43" s="3">
+        <v>44</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="G43" s="3">
+        <v>1</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="J43" s="3">
+        <v>1</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="Q43" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
+        <v>45</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0</v>
+      </c>
+      <c r="P44" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A45" s="3">
+        <v>46</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="4"/>
+      <c r="J45" s="3">
+        <v>0</v>
+      </c>
+      <c r="K45" s="4"/>
+      <c r="M45" s="3">
+        <v>0</v>
+      </c>
+      <c r="N45" s="4"/>
+      <c r="P45" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q45" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A46" s="3">
+        <v>47</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="3">
+        <v>1</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="M46" s="3">
+        <v>0</v>
+      </c>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q46" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A47" s="3">
+        <v>48</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="4"/>
+      <c r="J47" s="3">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4"/>
+      <c r="M47" s="3">
+        <v>0</v>
+      </c>
+      <c r="N47" s="4"/>
+      <c r="P47" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q47" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A48" s="3">
+        <v>49</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="3">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="3">
+        <v>0</v>
+      </c>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A49" s="3">
+        <v>50</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="3">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="3">
+        <v>0</v>
+      </c>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q49" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A50" s="3">
+        <v>51</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="4"/>
+      <c r="J50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4"/>
+      <c r="M50" s="3">
+        <v>0</v>
+      </c>
+      <c r="N50" s="4"/>
+      <c r="P50" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q50" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A51" s="3">
+        <v>53</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="3">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="3">
+        <v>0</v>
+      </c>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q51" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A52" s="3">
+        <v>54</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0</v>
+      </c>
+      <c r="M52" s="3">
+        <v>0</v>
+      </c>
+      <c r="P52" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q52" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A53" s="3">
+        <v>55</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="4"/>
+      <c r="J53" s="3">
+        <v>0</v>
+      </c>
+      <c r="K53" s="4"/>
+      <c r="M53" s="3">
+        <v>1</v>
+      </c>
+      <c r="N53" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O53" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="P53" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q53" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A54" s="3">
+        <v>56</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="J54" s="3">
+        <v>0</v>
+      </c>
+      <c r="M54" s="3">
+        <v>0</v>
+      </c>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q54" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="D55" s="3">
+        <f>SUM(D2:D54)</f>
+        <v>1</v>
+      </c>
+      <c r="G55" s="3">
+        <f>SUM(G2:G54)</f>
+        <v>3</v>
+      </c>
+      <c r="J55" s="3">
+        <f>SUM(J2:J54)</f>
+        <v>4</v>
+      </c>
+      <c r="M55" s="3">
+        <f>SUM(M2:M54)</f>
+        <v>3</v>
+      </c>
+      <c r="P55" s="3">
+        <f>SUM(G55:M55)</f>
+        <v>10</v>
+      </c>
+      <c r="Q55" s="3">
+        <f>SUM(Q2:Q54)</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FC520E-C64D-6242-ADD9-027A4DCE44BD}">
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46:XFD49"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12427,379 +14555,6 @@
     <sortCondition ref="A1:A64"/>
     <sortCondition ref="B1:B64"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393A85D5-950D-1643-BDA0-003D891BE10F}">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="4" width="10.83203125" style="13"/>
-    <col min="5" max="5" width="16" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="13"/>
-    <col min="7" max="7" width="43.33203125" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>419</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>424</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>426</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>429</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>431</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>286</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13026,4 +14781,377 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5A1989-7DD3-014D-B7BA-CCA42A69779F}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="13"/>
+    <col min="5" max="5" width="16" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="13"/>
+    <col min="7" max="7" width="43.33203125" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>